<commit_message>
updaterad projektplan och gantt-scheman
</commit_message>
<xml_diff>
--- a/Documents/ProjectC4_Gantt_Milestones.xlsx
+++ b/Documents/ProjectC4_Gantt_Milestones.xlsx
@@ -81,9 +81,6 @@
     <t xml:space="preserve">    Sammanställning</t>
   </si>
   <si>
-    <t>Hanledningsmöten</t>
-  </si>
-  <si>
     <t>Rolf</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Testning och testrapport</t>
+  </si>
+  <si>
+    <t>Handledningsmöten</t>
   </si>
 </sst>
 </file>
@@ -725,13 +725,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" customWidth="1"/>
     <col min="2" max="2" width="7.453125" customWidth="1"/>
     <col min="3" max="3" width="9.453125" customWidth="1"/>
     <col min="5" max="16" width="3.54296875" style="1" customWidth="1"/>
@@ -795,16 +795,16 @@
     </row>
     <row r="3" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" s="14">
         <v>5</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -847,10 +847,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="4"/>
@@ -873,10 +873,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
@@ -899,10 +899,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
@@ -925,10 +925,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -989,10 +989,10 @@
         <v>110</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -1015,10 +1015,10 @@
         <v>30</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
@@ -1041,10 +1041,10 @@
         <v>100</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
@@ -1067,10 +1067,10 @@
         <v>100</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1093,10 +1093,10 @@
         <v>80</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1119,10 +1119,10 @@
         <v>110</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1145,10 +1145,10 @@
         <v>110</v>
       </c>
       <c r="C17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>23</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>24</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1171,10 +1171,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1209,16 +1209,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <v>30</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -1259,10 +1259,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>

</xml_diff>

<commit_message>
update: gantt_milestone, gantt_participants, projectplan, requirements
</commit_message>
<xml_diff>
--- a/Documents/ProjectC4_Gantt_Milestones.xlsx
+++ b/Documents/ProjectC4_Gantt_Milestones.xlsx
@@ -352,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,11 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -419,6 +415,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,10 +799,10 @@
       <c r="B3" s="14">
         <v>5</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="31" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="15"/>
@@ -846,10 +845,10 @@
       <c r="B5" s="2">
         <v>15</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="5"/>
@@ -872,10 +871,10 @@
       <c r="B6" s="2">
         <v>15</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="5"/>
@@ -898,10 +897,10 @@
       <c r="B7" s="2">
         <v>15</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="5"/>
@@ -924,10 +923,10 @@
       <c r="B8" s="2">
         <v>20</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="4"/>
@@ -988,10 +987,10 @@
       <c r="B11" s="2">
         <v>110</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="25" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="6"/>
@@ -1014,10 +1013,10 @@
       <c r="B12" s="2">
         <v>30</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="27" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="4"/>
@@ -1040,10 +1039,10 @@
       <c r="B13" s="2">
         <v>100</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="6"/>
@@ -1066,10 +1065,10 @@
       <c r="B14" s="2">
         <v>100</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="25" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="4"/>
@@ -1092,10 +1091,10 @@
       <c r="B15" s="2">
         <v>80</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="4"/>
@@ -1118,10 +1117,10 @@
       <c r="B16" s="2">
         <v>110</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="27" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="4"/>
@@ -1144,10 +1143,10 @@
       <c r="B17" s="2">
         <v>110</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="4"/>
@@ -1170,10 +1169,10 @@
       <c r="B18" s="2">
         <v>20</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4"/>
@@ -1214,10 +1213,10 @@
       <c r="B20" s="2">
         <v>30</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="4"/>
@@ -1228,7 +1227,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="4"/>
       <c r="P20" s="19"/>
@@ -1256,12 +1255,12 @@
         <v>16</v>
       </c>
       <c r="B22" s="21">
-        <v>20</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="22"/>
@@ -1272,10 +1271,10 @@
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
       <c r="O22" s="23"/>
-      <c r="P22" s="24"/>
+      <c r="P22" s="32"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
@@ -1283,7 +1282,7 @@
       </c>
       <c r="B23" s="12" t="str">
         <f>SUM(B3:B22) &amp;" h"</f>
-        <v>780 h</v>
+        <v>790 h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>